<commit_message>
Version 7.5 mejoras al codigo
</commit_message>
<xml_diff>
--- a/resultados/resultado_version 12.xlsx
+++ b/resultados/resultado_version 12.xlsx
@@ -596,17 +596,17 @@
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>easy:80.8</t>
+          <t>easy:81.62</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>very:13.79</t>
+          <t>very:13.31</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>neutral:5.01</t>
+          <t>neutral:4.69</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>None:None</t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -681,17 +681,17 @@
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>easy:87.26</t>
+          <t>easy:87.43</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>very:8.23</t>
+          <t>very:8.17</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>neutral:4.02</t>
+          <t>neutral:3.93</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>difficult:0.08</t>
+          <t>difficult:0.07</t>
         </is>
       </c>
     </row>

</xml_diff>